<commit_message>
use log returns for skew and kurtosis
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -932,28 +932,28 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>-0.6899999999999999</v>
+        <v>-0.78</v>
       </c>
       <c r="C10">
-        <v>-0.57</v>
+        <v>-0.64</v>
       </c>
       <c r="D10">
-        <v>-0.52</v>
+        <v>-0.59</v>
       </c>
       <c r="E10">
-        <v>-1.33</v>
+        <v>-1.51</v>
       </c>
       <c r="F10">
-        <v>-1.42</v>
+        <v>-1.59</v>
       </c>
       <c r="G10">
-        <v>0.35</v>
+        <v>0.06</v>
       </c>
       <c r="H10">
-        <v>-0.5600000000000001</v>
+        <v>-0.63</v>
       </c>
       <c r="I10">
-        <v>-1.21</v>
+        <v>-1.36</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -961,28 +961,28 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>4.29</v>
+        <v>4.64</v>
       </c>
       <c r="C11">
-        <v>3.72</v>
+        <v>3.88</v>
       </c>
       <c r="D11">
-        <v>3.56</v>
+        <v>3.68</v>
       </c>
       <c r="E11">
-        <v>12.21</v>
+        <v>14.07</v>
       </c>
       <c r="F11">
-        <v>12.49</v>
+        <v>14.4</v>
       </c>
       <c r="G11">
-        <v>20.97</v>
+        <v>19.27</v>
       </c>
       <c r="H11">
-        <v>3.96</v>
+        <v>4.1</v>
       </c>
       <c r="I11">
-        <v>10.27</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="12" spans="1:9">

</xml_diff>